<commit_message>
poi 导出 excel util包
</commit_message>
<xml_diff>
--- a/java-design-mode/interview.xlsx
+++ b/java-design-mode/interview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IdeaProjects\springboot3-learning\java-design-mode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CF028C-04FC-43F9-A10E-A1F1739153A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954E1A9C-71DA-4C37-9F2C-8EC2477ED054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="0" windowWidth="35370" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -591,9 +591,6 @@
     <t>What are the common injection methods in spring?</t>
   </si>
   <si>
-    <t>Why use spring boot?</t>
-  </si>
-  <si>
     <t>What is the difference between using Integer and int for mapping in hibernate?</t>
   </si>
   <si>
@@ -1604,12 +1601,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Struts Workflow</t>
-  </si>
-  <si>
-    <t>What are the ways to run Spring Boot?</t>
-  </si>
-  <si>
-    <t>Spring Boot Configuration Loading Order</t>
   </si>
   <si>
     <t>Spring Boot's Core Configuration Files</t>
@@ -1995,6 +1986,18 @@
   </si>
   <si>
     <t>Explain method overloading and method rewriting.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring Boot Configuration Loading Order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>What are the ways to run Spring Boot?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Why use spring boot?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2375,8 +2378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC6FBBB-F1B5-4500-BED7-1F56F5D931CD}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A205" sqref="A205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2387,7 +2390,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2395,131 +2398,131 @@
         <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B7" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B11" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B14" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B15" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B19" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2529,188 +2532,188 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B21" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B22" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B23" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B25" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B28" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B29" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B33" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B41" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B43" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B47" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2720,215 +2723,215 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B63" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B66" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B77" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B78" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B80" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B82" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -2938,90 +2941,90 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B96" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B97" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B100" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B101" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B102" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -3031,10 +3034,10 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B105" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -3042,7 +3045,7 @@
         <v>142</v>
       </c>
       <c r="B106" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -3052,22 +3055,22 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -3077,57 +3080,57 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B113" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B114" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B117" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B118" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B120" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -3137,17 +3140,17 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -3157,39 +3160,39 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B127" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B128" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B129" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B130" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -3197,94 +3200,94 @@
         <v>145</v>
       </c>
       <c r="B132" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B134" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B135" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B145" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
@@ -3294,55 +3297,55 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>146</v>
+        <v>537</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>426</v>
+        <v>536</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>427</v>
+        <v>535</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B152" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B153" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B155" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -3352,92 +3355,92 @@
     </row>
     <row r="157" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B158" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B159" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B160" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B161" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B162" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="B165" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B166" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B167" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B168" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -3447,111 +3450,111 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B177" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B179" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
@@ -3561,18 +3564,18 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B192" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B193" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
@@ -3587,12 +3590,12 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
@@ -3602,23 +3605,23 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B199" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B200" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
   </sheetData>
@@ -3651,7 +3654,7 @@
         <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3659,7 +3662,7 @@
         <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3667,23 +3670,23 @@
         <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" t="s">
         <v>288</v>
-      </c>
-      <c r="B6" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3699,7 +3702,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3712,7 +3715,7 @@
         <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3720,62 +3723,62 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
         <v>156</v>
-      </c>
-      <c r="B12" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B14" t="s">
         <v>286</v>
-      </c>
-      <c r="B14" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" t="s">
         <v>290</v>
-      </c>
-      <c r="B15" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B16" t="s">
         <v>292</v>
-      </c>
-      <c r="B16" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B19" t="s">
         <v>297</v>
-      </c>
-      <c r="B19" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3785,26 +3788,26 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B23" t="s">
         <v>233</v>
-      </c>
-      <c r="B23" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3817,7 +3820,7 @@
         <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3832,23 +3835,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" t="s">
         <v>227</v>
-      </c>
-      <c r="B28" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3863,10 +3866,10 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B33" t="s">
         <v>225</v>
-      </c>
-      <c r="B33" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="57" x14ac:dyDescent="0.2">
@@ -3874,7 +3877,7 @@
         <v>80</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3889,7 +3892,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -3909,10 +3912,10 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B41" t="s">
         <v>193</v>
-      </c>
-      <c r="B41" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -3925,23 +3928,23 @@
         <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -3954,7 +3957,7 @@
         <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3984,10 +3987,10 @@
     </row>
     <row r="53" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -4030,23 +4033,23 @@
         <v>111</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B62" t="s">
         <v>218</v>
-      </c>
-      <c r="B62" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -4059,7 +4062,7 @@
         <v>112</v>
       </c>
       <c r="B65" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -4079,10 +4082,10 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" t="s">
         <v>213</v>
-      </c>
-      <c r="B69" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -4105,7 +4108,7 @@
         <v>22</v>
       </c>
       <c r="B73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -4120,10 +4123,10 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" t="s">
         <v>220</v>
-      </c>
-      <c r="B76" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -4131,7 +4134,7 @@
         <v>128</v>
       </c>
       <c r="B77" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -4144,7 +4147,7 @@
         <v>126</v>
       </c>
       <c r="B79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -4157,12 +4160,12 @@
         <v>33</v>
       </c>
       <c r="B81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
@@ -4195,7 +4198,7 @@
         <v>124</v>
       </c>
       <c r="B88" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -4215,10 +4218,10 @@
     </row>
     <row r="92" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -4239,7 +4242,7 @@
         <v>114</v>
       </c>
       <c r="B95" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -4257,7 +4260,7 @@
         <v>41</v>
       </c>
       <c r="B98" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -4265,20 +4268,20 @@
         <v>40</v>
       </c>
       <c r="B99" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B100" t="s">
         <v>207</v>
-      </c>
-      <c r="B100" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -4288,10 +4291,10 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B103" t="s">
         <v>269</v>
-      </c>
-      <c r="B103" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -4299,12 +4302,12 @@
         <v>117</v>
       </c>
       <c r="B104" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -4334,23 +4337,23 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B111" t="s">
         <v>281</v>
-      </c>
-      <c r="B111" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B112" t="s">
         <v>283</v>
-      </c>
-      <c r="B112" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -4360,18 +4363,18 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B115" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B116" t="s">
         <v>202</v>
-      </c>
-      <c r="B116" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -4384,7 +4387,7 @@
         <v>104</v>
       </c>
       <c r="B118" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -4414,34 +4417,34 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B124" t="s">
         <v>248</v>
-      </c>
-      <c r="B124" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B125" t="s">
         <v>254</v>
-      </c>
-      <c r="B125" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B126" t="s">
         <v>258</v>
-      </c>
-      <c r="B126" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B127" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
@@ -4467,7 +4470,7 @@
         <v>99</v>
       </c>
       <c r="B131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -4475,15 +4478,15 @@
         <v>98</v>
       </c>
       <c r="B132" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -4523,20 +4526,20 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B143" t="s">
         <v>256</v>
-      </c>
-      <c r="B143" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -4561,95 +4564,95 @@
     </row>
     <row r="148" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B148" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="57" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B149" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="B149" s="5" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B150" t="s">
         <v>267</v>
-      </c>
-      <c r="B150" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B151" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B155" s="5" t="s">
         <v>261</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B156" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B157" t="s">
         <v>183</v>
-      </c>
-      <c r="B157" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B158" t="s">
         <v>177</v>
-      </c>
-      <c r="B158" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B159" t="s">
         <v>185</v>
-      </c>
-      <c r="B159" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
@@ -4657,7 +4660,7 @@
         <v>84</v>
       </c>
       <c r="B160" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
@@ -4670,7 +4673,7 @@
         <v>79</v>
       </c>
       <c r="B162" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
@@ -4680,26 +4683,26 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B164" t="s">
         <v>181</v>
-      </c>
-      <c r="B164" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B165" t="s">
         <v>179</v>
-      </c>
-      <c r="B165" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B166" t="s">
         <v>175</v>
-      </c>
-      <c r="B166" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
@@ -4742,7 +4745,7 @@
         <v>45</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
@@ -4750,7 +4753,7 @@
         <v>46</v>
       </c>
       <c r="B175" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
@@ -4763,22 +4766,22 @@
         <v>71</v>
       </c>
       <c r="B177" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
@@ -4788,12 +4791,12 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
@@ -4829,7 +4832,7 @@
         <v>52</v>
       </c>
       <c r="B190" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
@@ -4837,7 +4840,7 @@
         <v>51</v>
       </c>
       <c r="B191" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
@@ -4870,20 +4873,20 @@
         <v>57</v>
       </c>
       <c r="B197" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B198" t="s">
         <v>173</v>
-      </c>
-      <c r="B198" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>